<commit_message>
change cdel cost keys that calculate totals charts. tests passing
</commit_message>
<xml_diff>
--- a/tests/resources/cost_test_master_1_2020.xlsx
+++ b/tests/resources/cost_test_master_1_2020.xlsx
@@ -14539,7 +14539,7 @@
     <row r="651" ht="13.8" customHeight="1" s="9">
       <c r="A651" s="8" t="inlineStr">
         <is>
-          <t>Unprofiled CDEL Forecast Total</t>
+          <t>Unprofiled CDEL Forecast one off new costs</t>
         </is>
       </c>
       <c r="B651" s="8" t="n">
@@ -14803,7 +14803,7 @@
     <row r="663" ht="13.8" customHeight="1" s="9">
       <c r="A663" s="8" t="inlineStr">
         <is>
-          <t>Total CDEL Forecast Total</t>
+          <t>Total CDEL Forecast one off new costs</t>
         </is>
       </c>
       <c r="B663" s="8" t="n">

</xml_diff>

<commit_message>
all test cost profiles now out until 39-40
</commit_message>
<xml_diff>
--- a/tests/resources/cost_test_master_1_2020.xlsx
+++ b/tests/resources/cost_test_master_1_2020.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1228" uniqueCount="1024">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1229" uniqueCount="1024">
   <si>
     <t xml:space="preserve">Project/Programme Name</t>
   </si>
@@ -73,6 +73,9 @@
     <t xml:space="preserve">Re-baseline IPDC cost</t>
   </si>
   <si>
+    <t xml:space="preserve">Yes</t>
+  </si>
+  <si>
     <t xml:space="preserve">Re-baseline IPDC benefits</t>
   </si>
   <si>
@@ -116,9 +119,6 @@
   </si>
   <si>
     <t xml:space="preserve">Is your HMT Business case updated / approved annually by HMT or more frequently?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes</t>
   </si>
   <si>
     <t xml:space="preserve">Does the HMT Businesss Case cover the full life of the project?</t>
@@ -3301,9 +3301,9 @@
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A389" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C396" activeCellId="0" sqref="C396"/>
+      <selection pane="bottomLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3397,30 +3397,33 @@
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="B8" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>8</v>
@@ -3437,41 +3440,41 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C14" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E14" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C16" s="2" t="n">
         <v>42551</v>
@@ -3488,12 +3491,12 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>11</v>
@@ -3505,7 +3508,7 @@
         <v>11</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3513,16 +3516,16 @@
         <v>33</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3545,16 +3548,16 @@
         <v>37</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3575,16 +3578,16 @@
         <v>41</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3623,16 +3626,16 @@
         <v>11</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3670,7 +3673,7 @@
         <v>11</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3717,16 +3720,16 @@
         <v>61</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>11</v>
@@ -3737,10 +3740,10 @@
         <v>62</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>11</v>
@@ -3779,13 +3782,13 @@
         <v>11</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3821,13 +3824,13 @@
         <v>73</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>11</v>
@@ -3866,10 +3869,10 @@
         <v>11</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3880,7 +3883,7 @@
         <v>11</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3899,16 +3902,16 @@
         <v>79</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3933,19 +3936,19 @@
         <v>81</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3996,13 +3999,13 @@
         <v>11</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4067,19 +4070,19 @@
         <v>90</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4087,16 +4090,16 @@
         <v>91</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4104,19 +4107,19 @@
         <v>92</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -21574,13 +21577,13 @@
         <v>11</v>
       </c>
       <c r="C943" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="D943" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E943" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="F943" s="1" t="s">
         <v>11</v>
@@ -21594,13 +21597,13 @@
         <v>11</v>
       </c>
       <c r="C944" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="D944" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E944" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="F944" s="1" t="s">
         <v>11</v>
@@ -21645,7 +21648,7 @@
         <v>1010</v>
       </c>
       <c r="B947" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="D947" s="1" t="s">
         <v>11</v>
@@ -21659,7 +21662,7 @@
         <v>1011</v>
       </c>
       <c r="B948" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="C948" s="1" t="s">
         <v>11</v>
@@ -21679,7 +21682,7 @@
         <v>1012</v>
       </c>
       <c r="B949" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="D949" s="1" t="s">
         <v>11</v>
@@ -21693,7 +21696,7 @@
         <v>1013</v>
       </c>
       <c r="B950" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="C950" s="1" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
tidy of change_cost_keys inclusion of tests for programme. tests passing
</commit_message>
<xml_diff>
--- a/tests/resources/cost_test_master_1_2020.xlsx
+++ b/tests/resources/cost_test_master_1_2020.xlsx
@@ -21032,15 +21032,9 @@
           <t>16-17 Forecast one off new costs</t>
         </is>
       </c>
-      <c r="D945" t="n">
-        <v>4.09</v>
-      </c>
-      <c r="E945" t="n">
-        <v>0</v>
-      </c>
-      <c r="F945" t="n">
-        <v>11.36</v>
-      </c>
+      <c r="D945" s="7" t="n"/>
+      <c r="E945" s="7" t="n"/>
+      <c r="F945" s="7" t="n"/>
     </row>
     <row r="946" ht="13.8" customHeight="1" s="8">
       <c r="A946" s="13" t="inlineStr">
@@ -21048,13 +21042,13 @@
           <t>16-17 RDEL Actual recurring new costs</t>
         </is>
       </c>
-      <c r="D946" t="n">
-        <v>0</v>
-      </c>
-      <c r="E946" t="n">
-        <v>0</v>
-      </c>
-      <c r="F946" t="n">
+      <c r="D946" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E946" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F946" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -21064,13 +21058,13 @@
           <t>16-17 RDEL Actual recurring old costs</t>
         </is>
       </c>
-      <c r="D947" t="n">
-        <v>0</v>
-      </c>
-      <c r="E947" t="n">
-        <v>0</v>
-      </c>
-      <c r="F947" t="n">
+      <c r="D947" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E947" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F947" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -21080,16 +21074,16 @@
           <t>16-17 RDEL Actual Total</t>
         </is>
       </c>
-      <c r="C948" t="n">
-        <v>0</v>
-      </c>
-      <c r="D948" t="n">
+      <c r="C948" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D948" s="7" t="n">
         <v>4.09</v>
       </c>
-      <c r="E948" t="n">
-        <v>0</v>
-      </c>
-      <c r="F948" t="n">
+      <c r="E948" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F948" s="7" t="n">
         <v>11.36</v>
       </c>
     </row>
@@ -21120,16 +21114,16 @@
           <t>16-17 CDEL Actual Total</t>
         </is>
       </c>
-      <c r="C952" t="n">
-        <v>0</v>
-      </c>
-      <c r="D952" t="n">
-        <v>0</v>
-      </c>
-      <c r="E952" t="n">
-        <v>0</v>
-      </c>
-      <c r="F952" t="n">
+      <c r="C952" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D952" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E952" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F952" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -21146,13 +21140,13 @@
           <t>17-18 RDEL Forecast one off new costs</t>
         </is>
       </c>
-      <c r="D954" t="n">
+      <c r="D954" s="7" t="n">
         <v>12</v>
       </c>
-      <c r="E954" t="n">
-        <v>0</v>
-      </c>
-      <c r="F954" t="n">
+      <c r="E954" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F954" s="7" t="n">
         <v>46.72</v>
       </c>
     </row>
@@ -21162,10 +21156,10 @@
           <t>17-18 RDEL Forecast recurring new costs</t>
         </is>
       </c>
-      <c r="E955" t="n">
-        <v>0</v>
-      </c>
-      <c r="F955" t="n">
+      <c r="E955" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F955" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -21175,13 +21169,13 @@
           <t>17-18 RDEL Forecast recurring old costs</t>
         </is>
       </c>
-      <c r="D956" t="n">
-        <v>0</v>
-      </c>
-      <c r="E956" t="n">
-        <v>0</v>
-      </c>
-      <c r="F956" t="n">
+      <c r="D956" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E956" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F956" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -21191,16 +21185,16 @@
           <t>17-18 RDEL Forecast Total</t>
         </is>
       </c>
-      <c r="C957" t="n">
-        <v>0</v>
-      </c>
-      <c r="D957" t="n">
+      <c r="C957" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D957" s="7" t="n">
         <v>12</v>
       </c>
-      <c r="E957" t="n">
-        <v>0</v>
-      </c>
-      <c r="F957" t="n">
+      <c r="E957" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F957" s="7" t="n">
         <v>46.72</v>
       </c>
     </row>
@@ -21210,16 +21204,16 @@
           <t>17-18 CDEL Forecast one off new costs</t>
         </is>
       </c>
-      <c r="C958" t="n">
+      <c r="C958" s="7" t="n">
         <v>379.5</v>
       </c>
-      <c r="D958" t="n">
+      <c r="D958" s="7" t="n">
         <v>174</v>
       </c>
-      <c r="E958" t="n">
+      <c r="E958" s="7" t="n">
         <v>49.9</v>
       </c>
-      <c r="F958" t="n">
+      <c r="F958" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -21229,13 +21223,13 @@
           <t>17-18 CDEL Forecast recurring new costs</t>
         </is>
       </c>
-      <c r="C959" t="n">
-        <v>0</v>
-      </c>
-      <c r="E959" t="n">
-        <v>0</v>
-      </c>
-      <c r="F959" t="n">
+      <c r="C959" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E959" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F959" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -21245,16 +21239,16 @@
           <t>17-18 CDEL Forecast recurring old costs</t>
         </is>
       </c>
-      <c r="C960" t="n">
-        <v>0</v>
-      </c>
-      <c r="D960" t="n">
-        <v>0</v>
-      </c>
-      <c r="E960" t="n">
-        <v>0</v>
-      </c>
-      <c r="F960" t="n">
+      <c r="C960" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D960" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E960" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F960" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -21264,16 +21258,16 @@
           <t>17-18 CDEL Forecast one off new costs</t>
         </is>
       </c>
-      <c r="C961" t="n">
+      <c r="C961" s="7" t="n">
         <v>379.5</v>
       </c>
-      <c r="D961" t="n">
+      <c r="D961" s="7" t="n">
         <v>174</v>
       </c>
-      <c r="E961" t="n">
+      <c r="E961" s="7" t="n">
         <v>49.9</v>
       </c>
-      <c r="F961" t="n">
+      <c r="F961" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -21283,10 +21277,10 @@
           <t>17-18 Forecast Non-Gov</t>
         </is>
       </c>
-      <c r="D962" t="n">
+      <c r="D962" s="7" t="n">
         <v>96</v>
       </c>
-      <c r="F962" t="n">
+      <c r="F962" s="7" t="n">
         <v>174.7</v>
       </c>
     </row>
@@ -21296,13 +21290,13 @@
           <t>18-19 RDEL Forecast one off new costs</t>
         </is>
       </c>
-      <c r="D963" t="n">
+      <c r="D963" s="7" t="n">
         <v>37.88</v>
       </c>
-      <c r="E963" t="n">
-        <v>0</v>
-      </c>
-      <c r="F963" t="n">
+      <c r="E963" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F963" s="7" t="n">
         <v>36.22</v>
       </c>
     </row>
@@ -21312,10 +21306,10 @@
           <t>18-19 RDEL Forecast recurring new costs</t>
         </is>
       </c>
-      <c r="E964" t="n">
-        <v>0</v>
-      </c>
-      <c r="F964" t="n">
+      <c r="E964" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F964" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -21325,13 +21319,13 @@
           <t>18-19 RDEL Forecast recurring old costs</t>
         </is>
       </c>
-      <c r="D965" t="n">
-        <v>0</v>
-      </c>
-      <c r="E965" t="n">
-        <v>0</v>
-      </c>
-      <c r="F965" t="n">
+      <c r="D965" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E965" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F965" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -21341,16 +21335,16 @@
           <t>18-19 RDEL Forecast Non Gov costs</t>
         </is>
       </c>
-      <c r="C966" t="n">
-        <v>0</v>
-      </c>
-      <c r="D966" t="n">
-        <v>0</v>
-      </c>
-      <c r="E966" t="n">
-        <v>0</v>
-      </c>
-      <c r="F966" t="n">
+      <c r="C966" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D966" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E966" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F966" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -21360,16 +21354,16 @@
           <t>18-19 RDEL Forecast Total</t>
         </is>
       </c>
-      <c r="C967" t="n">
-        <v>0</v>
-      </c>
-      <c r="D967" t="n">
+      <c r="C967" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D967" s="7" t="n">
         <v>37.88</v>
       </c>
-      <c r="E967" t="n">
-        <v>0</v>
-      </c>
-      <c r="F967" t="n">
+      <c r="E967" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F967" s="7" t="n">
         <v>36.22</v>
       </c>
     </row>
@@ -21379,16 +21373,16 @@
           <t>18-19 RDEL Forecast Income</t>
         </is>
       </c>
-      <c r="C968" t="n">
-        <v>0</v>
-      </c>
-      <c r="D968" t="n">
-        <v>0</v>
-      </c>
-      <c r="E968" t="n">
-        <v>0</v>
-      </c>
-      <c r="F968" t="n">
+      <c r="C968" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D968" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E968" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F968" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -21398,16 +21392,16 @@
           <t>18-19 CDEL Forecast one off new costs</t>
         </is>
       </c>
-      <c r="C969" t="n">
+      <c r="C969" s="7" t="n">
         <v>470</v>
       </c>
-      <c r="D969" t="n">
+      <c r="D969" s="7" t="n">
         <v>25</v>
       </c>
-      <c r="E969" t="n">
+      <c r="E969" s="7" t="n">
         <v>61.9</v>
       </c>
-      <c r="F969" t="n">
+      <c r="F969" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -21417,13 +21411,13 @@
           <t>18-19 CDEL Forecast recurring new costs</t>
         </is>
       </c>
-      <c r="C970" t="n">
-        <v>0</v>
-      </c>
-      <c r="E970" t="n">
-        <v>0</v>
-      </c>
-      <c r="F970" t="n">
+      <c r="C970" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E970" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F970" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -21433,16 +21427,16 @@
           <t>18-19 CDEL Forecast recurring old costs</t>
         </is>
       </c>
-      <c r="C971" t="n">
-        <v>0</v>
-      </c>
-      <c r="D971" t="n">
-        <v>0</v>
-      </c>
-      <c r="E971" t="n">
-        <v>0</v>
-      </c>
-      <c r="F971" t="n">
+      <c r="C971" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D971" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E971" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F971" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -21452,10 +21446,10 @@
           <t>18-19 Forecast Non-Gov</t>
         </is>
       </c>
-      <c r="D972" t="n">
+      <c r="D972" s="7" t="n">
         <v>96</v>
       </c>
-      <c r="F972" t="n">
+      <c r="F972" s="7" t="n">
         <v>71.09999999999999</v>
       </c>
     </row>
@@ -21465,16 +21459,16 @@
           <t>18-19 CDEL Forecast Total WLC</t>
         </is>
       </c>
-      <c r="C973" t="n">
+      <c r="C973" s="7" t="n">
         <v>447.8</v>
       </c>
-      <c r="D973" t="n">
+      <c r="D973" s="7" t="n">
         <v>110.25</v>
       </c>
-      <c r="E973" t="n">
+      <c r="E973" s="7" t="n">
         <v>78.40000000000001</v>
       </c>
-      <c r="F973" t="n">
+      <c r="F973" s="7" t="n">
         <v>99.90000000000001</v>
       </c>
     </row>
@@ -21484,7 +21478,7 @@
           <t>18-19 Forecast - Income both Revenue and Capital</t>
         </is>
       </c>
-      <c r="F974" t="n">
+      <c r="F974" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -21494,16 +21488,16 @@
           <t>19-20 RDEL Forecast one off new costs</t>
         </is>
       </c>
-      <c r="B975" t="n">
-        <v>0</v>
-      </c>
-      <c r="D975" t="n">
+      <c r="B975" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D975" s="7" t="n">
         <v>34.49</v>
       </c>
-      <c r="E975" t="n">
-        <v>0</v>
-      </c>
-      <c r="F975" t="n">
+      <c r="E975" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F975" s="7" t="n">
         <v>33.42</v>
       </c>
     </row>
@@ -21513,13 +21507,13 @@
           <t>19-20 RDEL Forecast recurring new costs</t>
         </is>
       </c>
-      <c r="B976" t="n">
-        <v>0</v>
-      </c>
-      <c r="E976" t="n">
-        <v>0</v>
-      </c>
-      <c r="F976" t="n">
+      <c r="B976" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E976" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F976" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -21529,16 +21523,16 @@
           <t>19-20 RDEL Forecast recurring old costs</t>
         </is>
       </c>
-      <c r="B977" t="n">
-        <v>0</v>
-      </c>
-      <c r="D977" t="n">
-        <v>0</v>
-      </c>
-      <c r="E977" t="n">
-        <v>0</v>
-      </c>
-      <c r="F977" t="n">
+      <c r="B977" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D977" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E977" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F977" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -21548,19 +21542,19 @@
           <t>19-20 RDEL Forecast Non Gov costs</t>
         </is>
       </c>
-      <c r="B978" t="n">
-        <v>0</v>
-      </c>
-      <c r="C978" t="n">
-        <v>0</v>
-      </c>
-      <c r="D978" t="n">
-        <v>0</v>
-      </c>
-      <c r="E978" t="n">
-        <v>0</v>
-      </c>
-      <c r="F978" t="n">
+      <c r="B978" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C978" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D978" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E978" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F978" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -21570,19 +21564,19 @@
           <t>19-20 RDEL Forecast Total</t>
         </is>
       </c>
-      <c r="B979" t="n">
-        <v>0</v>
-      </c>
-      <c r="C979" t="n">
-        <v>0</v>
-      </c>
-      <c r="D979" t="n">
+      <c r="B979" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C979" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D979" s="7" t="n">
         <v>34.49</v>
       </c>
-      <c r="E979" t="n">
-        <v>0</v>
-      </c>
-      <c r="F979" t="n">
+      <c r="E979" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F979" s="7" t="n">
         <v>33.42</v>
       </c>
     </row>
@@ -21592,19 +21586,19 @@
           <t>19-20 RDEL Forecast Income</t>
         </is>
       </c>
-      <c r="B980" t="n">
-        <v>0</v>
-      </c>
-      <c r="C980" t="n">
-        <v>0</v>
-      </c>
-      <c r="D980" t="n">
-        <v>0</v>
-      </c>
-      <c r="E980" t="n">
-        <v>0</v>
-      </c>
-      <c r="F980" t="n">
+      <c r="B980" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C980" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D980" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E980" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F980" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -21614,19 +21608,19 @@
           <t>19-20 CDEL Forecast one off new costs</t>
         </is>
       </c>
-      <c r="B981" t="n">
-        <v>0</v>
-      </c>
-      <c r="C981" t="n">
+      <c r="B981" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C981" s="7" t="n">
         <v>243.9</v>
       </c>
-      <c r="D981" t="n">
-        <v>0</v>
-      </c>
-      <c r="E981" t="n">
+      <c r="D981" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E981" s="7" t="n">
         <v>64.3</v>
       </c>
-      <c r="F981" t="n">
+      <c r="F981" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -21636,19 +21630,19 @@
           <t>19-20 CDEL Forecast recurring new costs</t>
         </is>
       </c>
-      <c r="B982" t="n">
-        <v>0</v>
-      </c>
-      <c r="C982" t="n">
-        <v>0</v>
-      </c>
-      <c r="D982" t="n">
-        <v>0</v>
-      </c>
-      <c r="E982" t="n">
-        <v>0</v>
-      </c>
-      <c r="F982" t="n">
+      <c r="B982" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C982" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D982" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E982" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F982" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -21658,19 +21652,19 @@
           <t>19-20 CDEL Forecast recurring old costs</t>
         </is>
       </c>
-      <c r="B983" t="n">
-        <v>0</v>
-      </c>
-      <c r="C983" t="n">
-        <v>0</v>
-      </c>
-      <c r="D983" t="n">
-        <v>0</v>
-      </c>
-      <c r="E983" t="n">
-        <v>0</v>
-      </c>
-      <c r="F983" t="n">
+      <c r="B983" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C983" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D983" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E983" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F983" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -21680,13 +21674,13 @@
           <t>19-20 Forecast Non-Gov</t>
         </is>
       </c>
-      <c r="B984" t="n">
-        <v>0</v>
-      </c>
-      <c r="E984" t="n">
-        <v>0</v>
-      </c>
-      <c r="F984" t="n">
+      <c r="B984" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E984" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F984" s="7" t="n">
         <v>30.7</v>
       </c>
     </row>
@@ -21696,19 +21690,19 @@
           <t>19-20 CDEL Forecast Total WLC</t>
         </is>
       </c>
-      <c r="B985" t="n">
-        <v>0</v>
-      </c>
-      <c r="C985" t="n">
+      <c r="B985" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C985" s="7" t="n">
         <v>320.9</v>
       </c>
-      <c r="D985" t="n">
-        <v>0</v>
-      </c>
-      <c r="E985" t="n">
+      <c r="D985" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E985" s="7" t="n">
         <v>165</v>
       </c>
-      <c r="F985" t="n">
+      <c r="F985" s="7" t="n">
         <v>11.7</v>
       </c>
     </row>
@@ -21718,10 +21712,10 @@
           <t>19-20 Forecast - Income both Revenue and Capital</t>
         </is>
       </c>
-      <c r="B986" t="n">
-        <v>0</v>
-      </c>
-      <c r="F986" t="n">
+      <c r="B986" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F986" s="7" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
refactoring of ipdc_dashboard_code. financial part done
</commit_message>
<xml_diff>
--- a/tests/resources/cost_test_master_1_2020.xlsx
+++ b/tests/resources/cost_test_master_1_2020.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1206" uniqueCount="1040">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1214" uniqueCount="1042">
   <si>
     <t xml:space="preserve">Project/Programme Name</t>
   </si>
@@ -3140,6 +3140,12 @@
   </si>
   <si>
     <t xml:space="preserve">Blue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project stage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amber/Red</t>
   </si>
 </sst>
 </file>
@@ -3224,7 +3230,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3250,6 +3256,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3332,10 +3342,10 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A980" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="D995" activeCellId="0" sqref="D995"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A977" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="C987" activeCellId="0" sqref="C987"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -22241,6 +22251,34 @@
       </c>
       <c r="F987" s="1" t="s">
         <v>1039</v>
+      </c>
+    </row>
+    <row r="988" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A988" s="7" t="s">
+        <v>1040</v>
+      </c>
+      <c r="B988" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="989" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A989" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B989" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C989" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D989" s="1" t="s">
+        <v>1041</v>
+      </c>
+      <c r="E989" s="1" t="s">
+        <v>1038</v>
+      </c>
+      <c r="F989" s="1" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="1047105" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
refactor Benefits class and graphs so in line with latest data structure
</commit_message>
<xml_diff>
--- a/tests/resources/cost_test_master_1_2020.xlsx
+++ b/tests/resources/cost_test_master_1_2020.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1214" uniqueCount="1042">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1215" uniqueCount="1043">
   <si>
     <t xml:space="preserve">Project/Programme Name</t>
   </si>
@@ -3146,6 +3146,9 @@
   </si>
   <si>
     <t xml:space="preserve">Amber/Red</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GMPP - IPA ID Number</t>
   </si>
 </sst>
 </file>
@@ -3345,7 +3348,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A977" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C987" activeCellId="0" sqref="C987"/>
+      <selection pane="bottomLeft" activeCell="B994" activeCellId="0" sqref="B994"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -22279,6 +22282,11 @@
       </c>
       <c r="F989" s="1" t="s">
         <v>103</v>
+      </c>
+    </row>
+    <row r="990" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A990" s="1" t="s">
+        <v>1042</v>
       </c>
     </row>
     <row r="1047105" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>